<commit_message>
add tasks to utils
</commit_message>
<xml_diff>
--- a/circles/excel/задачиПримерыИванов.xlsx
+++ b/circles/excel/задачиПримерыИванов.xlsx
@@ -75,7 +75,7 @@
     <t xml:space="preserve">430;480;390;700;910;800</t>
   </si>
   <si>
-    <t xml:space="preserve">(Гаджеты|Док-станция)&amp;Часы</t>
+    <t xml:space="preserve">(Гаджеты|Часы)&amp;Док-станция</t>
   </si>
   <si>
     <t xml:space="preserve">Валюта;Кредит;Рынок;Рынок|Валюта;Кредит&amp;(Рынок&amp;Валюта);Валюта|Кредит</t>
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -895,7 +895,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +921,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add constructor tasks to utils
</commit_message>
<xml_diff>
--- a/circles/excel/задачиПримерыИванов.xlsx
+++ b/circles/excel/задачиПримерыИванов.xlsx
@@ -84,10 +84,10 @@
     <t xml:space="preserve">290;230;350;500;90;460</t>
   </si>
   <si>
-    <t xml:space="preserve">Рынок&amp;(Валюта|Кредит)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Модель;Технология;Патент ;Патент|Модель;Технология&amp;(Патент|Модель);Патент&amp;(Модель|Технология)</t>
+    <t xml:space="preserve">Валюта&amp;(Рынок|Кредит)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модель;Технология;Патент;Патент|Модель;Технология&amp;(Патент|Модель);Патент&amp;(Модель|Технология)</t>
   </si>
   <si>
     <t xml:space="preserve">Модель|Технология</t>
@@ -96,7 +96,7 @@
     <t xml:space="preserve">Грибы;Рыжики;Фото;Рыжики|Фото;Грибы&amp;Фото;(Рыжики|Фото)&amp;Грибы</t>
   </si>
   <si>
-    <t xml:space="preserve">Грибы&amp;Рыжики</t>
+    <t xml:space="preserve">(Грибы|Фото)&amp;Рыжики</t>
   </si>
   <si>
     <t xml:space="preserve">Человек;Первобытный;Археология;Человек|Археология;Человек&amp;Первобытный;Археология&amp;Первобытный</t>
@@ -117,7 +117,7 @@
     <t xml:space="preserve">Парус&amp;Рында</t>
   </si>
   <si>
-    <t xml:space="preserve">Кот;Дикий;Гепард;Кот|Дикий; Дикий&amp;Кот&amp;Гепард;Гепард|Кот</t>
+    <t xml:space="preserve">Кот;Дикий;Гепард;Кот|Дикий;Дикий&amp;Кот&amp;Гепард;Гепард|Кот</t>
   </si>
   <si>
     <t xml:space="preserve">Кот&amp;(Дикий|Гепард)</t>
@@ -286,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>